<commit_message>
remove error decision Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/ExternalSources/Main_ex.xlsx
+++ b/DESIGN/rules/ExternalSources/Main_ex.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jandelahoz/Downloads/"/>
     </mc:Choice>
@@ -107,6 +107,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="9">
     <font>
       <sz val="10"/>
@@ -687,9 +688,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="3" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="12.5" collapsed="false"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="11.1640625" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="34.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="29" spans="2:5">
@@ -780,12 +781,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="2:5">
-      <c r="B37" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="9"/>
-    </row>
+    <row r="37" spans="2:5"/>
     <row r="38" spans="2:5" s="7" customFormat="1">
       <c r="B38" s="11"/>
       <c r="C38" s="12"/>
@@ -855,7 +851,6 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B37:C37"/>
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="B29:E29"/>
   </mergeCells>

</xml_diff>

<commit_message>
change range Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/ExternalSources/Main_ex.xlsx
+++ b/DESIGN/rules/ExternalSources/Main_ex.xlsx
@@ -536,10 +536,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="12.5" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="17.0" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.1640625" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="34.0" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="12.5" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.1640625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="29" spans="2:5" x14ac:dyDescent="0.15">
@@ -623,8 +623,8 @@
       <c r="C35" s="2">
         <v>1000000001</v>
       </c>
-      <c r="D35" s="2">
-        <v>1019999999</v>
+      <c r="D35" s="2" t="n">
+        <v>2.019999999E9</v>
       </c>
       <c r="E35" s="2">
         <v>80</v>

</xml_diff>